<commit_message>
Adding mutable data with executable step
</commit_message>
<xml_diff>
--- a/YagnaIQ_PageObject/TestData/TestData.xlsx
+++ b/YagnaIQ_PageObject/TestData/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -47,7 +47,37 @@
     <t>Test</t>
   </si>
   <si>
-    <t>tuhar@test.com</t>
+    <t>tuhar20@test.com</t>
+  </si>
+  <si>
+    <t>tuhar30@test.com</t>
+  </si>
+  <si>
+    <t>tuhar40@test.com</t>
+  </si>
+  <si>
+    <t>tuhar50@test.com</t>
+  </si>
+  <si>
+    <t>tuhar60@test.com</t>
+  </si>
+  <si>
+    <t>tuhar70@test.com</t>
+  </si>
+  <si>
+    <t>tuhar80@test.com</t>
+  </si>
+  <si>
+    <t>tuhar90@test.com</t>
+  </si>
+  <si>
+    <t>tuhar100@test.com</t>
+  </si>
+  <si>
+    <t>tuhar110@test.com</t>
+  </si>
+  <si>
+    <t>tuhar120@test.com</t>
   </si>
 </sst>
 </file>
@@ -55,10 +85,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -71,6 +101,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -86,14 +124,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -101,21 +131,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,15 +152,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -146,7 +183,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,16 +213,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,25 +235,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -228,67 +258,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,109 +432,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,6 +443,63 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -427,30 +514,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -472,39 +535,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -518,148 +548,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -667,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1014,13 +1044,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
     <col min="5" max="5" width="9.3"/>
   </cols>
@@ -1059,9 +1089,189 @@
         <v>13213131</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>13213132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>13213133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>13213134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>13213135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>13213136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>13213137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>13213138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>13213139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>13213140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>13213141</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="tuhar@test.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="tuhar20@test.com" tooltip="mailto:tuhar20@test.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="tuhar30@test.com" tooltip="mailto:tuhar30@test.com"/>
+    <hyperlink ref="D4" r:id="rId1" display="tuhar40@test.com" tooltip="mailto:tuhar20@test.com"/>
+    <hyperlink ref="D5" r:id="rId2" display="tuhar50@test.com" tooltip="mailto:tuhar30@test.com"/>
+    <hyperlink ref="D6" r:id="rId1" display="tuhar60@test.com" tooltip="mailto:tuhar20@test.com"/>
+    <hyperlink ref="D10" r:id="rId1" display="tuhar100@test.com" tooltip="mailto:tuhar20@test.com"/>
+    <hyperlink ref="D7" r:id="rId2" display="tuhar70@test.com" tooltip="mailto:tuhar30@test.com"/>
+    <hyperlink ref="D11" r:id="rId2" display="tuhar110@test.com" tooltip="mailto:tuhar30@test.com"/>
+    <hyperlink ref="D8" r:id="rId1" display="tuhar80@test.com" tooltip="mailto:tuhar20@test.com"/>
+    <hyperlink ref="D12" r:id="rId1" display="tuhar120@test.com" tooltip="mailto:tuhar20@test.com"/>
+    <hyperlink ref="D9" r:id="rId2" display="tuhar90@test.com" tooltip="mailto:tuhar30@test.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>